<commit_message>
Line chart - Add CompletedDate in task table for savinf the date when the task was complelted - Add the line chart for each tasks completed by user and month - handleUpdate/CreateTask use a Consumer<TaskEdit> now - The PUT task return the task updated - Add label in PieChartStatus for just hovering but hide it with .hide-default-labels-chart - When fetch tasks, I set the date ( new Date(...)) with the value task.completedTask - Remove MOCKS
</commit_message>
<xml_diff>
--- a/backend/Exports/tasks.xlsx
+++ b/backend/Exports/tasks.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Libellé de la tâche</t>
   </si>
@@ -23,28 +23,16 @@
     <t>Status</t>
   </si>
   <si>
-    <t>ADD labelllllllll</t>
+    <t>Se préinscrire</t>
   </si>
   <si>
-    <t>Sanchez Beth</t>
+    <t>null</t>
+  </si>
+  <si>
+    <t>En cours</t>
   </si>
   <si>
     <t>Terminé</t>
-  </si>
-  <si>
-    <t>Label 0</t>
-  </si>
-  <si>
-    <t>Jerry Smith</t>
-  </si>
-  <si>
-    <t>label 4</t>
-  </si>
-  <si>
-    <t>Morty Smith</t>
-  </si>
-  <si>
-    <t>En cours</t>
   </si>
 </sst>
 </file>
@@ -91,14 +79,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.450550079345703" customWidth="1"/>
-    <col min="2" max="2" width="12.421717643737793" customWidth="1"/>
+    <col min="2" max="2" width="10.398094177246094" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -126,24 +114,46 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ErrorSnackbar - Display an error snackbar every time a fetch failed - Fix bug null attribution /Excel tasks - Code clean up + optimize import
</commit_message>
<xml_diff>
--- a/backend/Exports/tasks.xlsx
+++ b/backend/Exports/tasks.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Libellé de la tâche</t>
   </si>
@@ -23,16 +23,25 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Se préinscrire</t>
+    <t>Discover</t>
   </si>
   <si>
-    <t>null</t>
+    <t>Sanchez Rick</t>
+  </si>
+  <si>
+    <t>Bloqué</t>
+  </si>
+  <si>
+    <t>Terminé</t>
+  </si>
+  <si>
+    <t>Label 1</t>
   </si>
   <si>
     <t>En cours</t>
   </si>
   <si>
-    <t>Terminé</t>
+    <t>Se préinscrire</t>
   </si>
 </sst>
 </file>
@@ -86,7 +95,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.450550079345703" customWidth="1"/>
-    <col min="2" max="2" width="10.398094177246094" customWidth="1"/>
+    <col min="2" max="2" width="11.877447128295898" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -125,35 +134,35 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>